<commit_message>
Generates test_predictions.csv file with columns [image_id, label, prediction, filename] sorted descending by prediction.
</commit_message>
<xml_diff>
--- a/README.kaggle.dataset.xlsx
+++ b/README.kaggle.dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t xml:space="preserve">bin2/test/0</t>
   </si>
@@ -69,12 +69,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +90,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,35 +204,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,15 +265,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.780612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,6 +361,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <f aca="false">C2+A2</f>
+        <v>48784</v>
+      </c>
       <c r="D4" s="0" t="n">
         <f aca="false">D3+B3</f>
         <v>65936</v>
@@ -445,6 +470,9 @@
       <c r="G16" s="0" t="n">
         <v>694</v>
       </c>
+      <c r="K16" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="0" t="n">
@@ -455,6 +483,14 @@
         <f aca="false">G15+G16</f>
         <v>17152</v>
       </c>
+      <c r="K17" s="2" t="n">
+        <v>61167</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="n">
+        <v>60000</v>
+      </c>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="n">
@@ -464,15 +500,41 @@
         <f aca="false">F17+G17</f>
         <v>88692</v>
       </c>
+      <c r="K18" s="5" t="n">
+        <v>15291</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>16458</v>
+      </c>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="n">
         <v>1660</v>
       </c>
+      <c r="K19" s="7" t="n">
+        <f aca="false">K17+K18</f>
+        <v>76458</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">M17+M18</f>
+        <v>76458</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <f aca="false">M19*0.8</f>
+        <v>61166.4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="n">
         <v>768</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="10" t="n">
+        <f aca="false">M19*0.2</f>
+        <v>15291.6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,10 +549,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="4" t="n">
@@ -498,7 +560,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="5" t="n">
+      <c r="F24" s="7" t="n">
         <v>63922</v>
       </c>
       <c r="G24" s="0" t="s">
@@ -509,7 +571,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="7" t="n">
         <v>15980</v>
       </c>
       <c r="H25" s="6" t="n">
@@ -518,18 +580,18 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="5" t="n">
+      <c r="F26" s="7" t="n">
         <v>8790</v>
       </c>
       <c r="H26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="7" t="n">
+      <c r="F27" s="8" t="n">
         <f aca="false">SUM(F24:F26)</f>
         <v>88692</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>